<commit_message>
Added Valuation Table and adjusted the DCF (Shifted upside cell to be in the B Column to make things easier to parse)
</commit_message>
<xml_diff>
--- a/Assignment Code/VEA_DCF.xlsx
+++ b/Assignment Code/VEA_DCF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmarogers/Library/Mobile Documents/com~apple~CloudDocs/Uni 2025/3422/Coding Part 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukec\Documents\2025 Sem 1\3422\Coding Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B258BA94-8DB9-9040-8EC3-8DAC3838370E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6D15F9-870E-49D8-AC26-C16005EA7512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{08537CD3-3619-8047-ABC8-88A44FE65EFC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{08537CD3-3619-8047-ABC8-88A44FE65EFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Getting FCFF" sheetId="1" r:id="rId1"/>
@@ -445,7 +445,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="3" builtinId="5"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -849,12 +849,12 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -874,7 +874,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -891,7 +891,7 @@
         <v>392.1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -911,7 +911,7 @@
         <v>384.9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -925,23 +925,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D642A58B-58A5-6447-8392-2E7517998A04}">
   <dimension ref="B1:Y89"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="119" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
     <col min="2" max="2" width="1.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="11" style="2"/>
     <col min="4" max="4" width="22.1640625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.58203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.08203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="20" width="11.33203125" style="2" customWidth="1"/>
     <col min="21" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -951,7 +952,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="2:23" ht="37" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
         <v>35</v>
       </c>
@@ -977,7 +978,7 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1001,7 +1002,7 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
     </row>
-    <row r="4" spans="2:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1027,7 +1028,7 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
     </row>
-    <row r="5" spans="2:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:23" ht="16" x14ac:dyDescent="0.4">
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
@@ -1055,7 +1056,7 @@
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -1083,7 +1084,7 @@
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>42</v>
       </c>
@@ -1111,7 +1112,7 @@
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
@@ -1140,7 +1141,7 @@
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1161,7 +1162,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1195,7 @@
       <c r="S10" s="15"/>
       <c r="T10" s="15"/>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1227,7 +1228,7 @@
       <c r="S11" s="16"/>
       <c r="T11" s="16"/>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1260,14 +1261,14 @@
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.35">
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B14" s="19" t="s">
         <v>11</v>
       </c>
@@ -1290,7 +1291,7 @@
       <c r="S14" s="20"/>
       <c r="T14" s="20"/>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
@@ -1311,7 +1312,7 @@
       <c r="S15" s="20"/>
       <c r="T15" s="20"/>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1325,7 +1326,7 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1338,7 +1339,7 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>37</v>
       </c>
@@ -1354,7 +1355,7 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1370,7 +1371,7 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
@@ -1387,7 +1388,7 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="E21" s="23"/>
       <c r="P21" s="1"/>
@@ -1396,7 +1397,7 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B22" s="19" t="s">
         <v>15</v>
       </c>
@@ -1419,7 +1420,7 @@
       <c r="S22" s="20"/>
       <c r="T22" s="20"/>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B24" s="26" t="s">
         <v>16</v>
       </c>
@@ -1442,7 +1443,7 @@
       <c r="S24" s="51"/>
       <c r="T24" s="51"/>
     </row>
-    <row r="25" spans="2:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:20" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B25" s="25"/>
       <c r="C25" s="2" t="s">
         <v>38</v>
@@ -1468,7 +1469,7 @@
       <c r="S25" s="28"/>
       <c r="T25" s="28"/>
     </row>
-    <row r="26" spans="2:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:20" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B26" s="25"/>
       <c r="C26" s="2" t="s">
         <v>39</v>
@@ -1494,7 +1495,7 @@
       <c r="S26" s="28"/>
       <c r="T26" s="28"/>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B27" s="25"/>
       <c r="C27" s="2" t="s">
         <v>40</v>
@@ -1525,7 +1526,7 @@
       <c r="S27" s="28"/>
       <c r="T27" s="28"/>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C28" s="2" t="s">
         <v>17</v>
       </c>
@@ -1552,7 +1553,7 @@
       <c r="S28" s="44"/>
       <c r="T28" s="44"/>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
         <v>18</v>
       </c>
@@ -1582,7 +1583,7 @@
       <c r="S29" s="53"/>
       <c r="T29" s="53"/>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B30" s="26" t="s">
         <v>19</v>
       </c>
@@ -1620,10 +1621,10 @@
       <c r="S30" s="51"/>
       <c r="T30" s="51"/>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.35">
       <c r="K31" s="31"/>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B32" s="32" t="s">
         <v>20</v>
       </c>
@@ -1636,7 +1637,7 @@
       </c>
       <c r="J32" s="35"/>
     </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
         <v>22</v>
       </c>
@@ -1681,7 +1682,7 @@
       <c r="V33" s="37"/>
       <c r="W33" s="37"/>
     </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B34" s="24" t="s">
         <v>23</v>
       </c>
@@ -1726,7 +1727,7 @@
       <c r="V34" s="39"/>
       <c r="W34" s="39"/>
     </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B35" s="40" t="s">
         <v>24</v>
       </c>
@@ -1765,7 +1766,7 @@
       </c>
       <c r="Q35" s="22"/>
     </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
         <v>25</v>
       </c>
@@ -1800,7 +1801,7 @@
       </c>
       <c r="Q36" s="11"/>
     </row>
-    <row r="37" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B37" s="24" t="s">
         <v>26</v>
       </c>
@@ -1845,7 +1846,7 @@
       <c r="W37" s="44"/>
       <c r="X37" s="35"/>
     </row>
-    <row r="38" spans="2:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B38" s="45" t="s">
         <v>20</v>
       </c>
@@ -1884,7 +1885,7 @@
       <c r="Q38" s="11"/>
       <c r="X38" s="23"/>
     </row>
-    <row r="39" spans="2:24" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="I39" s="22">
         <f>I38+0.05%</f>
         <v>7.5899999999999995E-2</v>
@@ -1912,7 +1913,7 @@
       </c>
       <c r="Q39" s="11"/>
     </row>
-    <row r="40" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B40" s="32" t="s">
         <v>27</v>
       </c>
@@ -1948,7 +1949,7 @@
       </c>
       <c r="Q40" s="11"/>
     </row>
-    <row r="41" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
         <v>28</v>
       </c>
@@ -1982,7 +1983,7 @@
       </c>
       <c r="Q41" s="11"/>
     </row>
-    <row r="42" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B42" s="2" t="s">
         <v>29</v>
       </c>
@@ -2016,7 +2017,7 @@
       </c>
       <c r="Q42" s="11"/>
     </row>
-    <row r="43" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B43" s="24" t="s">
         <v>30</v>
       </c>
@@ -2038,7 +2039,7 @@
       <c r="P43" s="11"/>
       <c r="Q43" s="11"/>
     </row>
-    <row r="44" spans="2:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B44" s="45" t="s">
         <v>31</v>
       </c>
@@ -2060,8 +2061,8 @@
       <c r="P44" s="11"/>
       <c r="Q44" s="11"/>
     </row>
-    <row r="45" spans="2:24" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B46" s="32" t="s">
         <v>32</v>
       </c>
@@ -2071,7 +2072,7 @@
       <c r="F46" s="32"/>
       <c r="G46" s="32"/>
     </row>
-    <row r="47" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B47" s="2" t="s">
         <v>12</v>
       </c>
@@ -2080,7 +2081,7 @@
         <v>1610000000</v>
       </c>
     </row>
-    <row r="48" spans="2:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B48" s="45" t="s">
         <v>33</v>
       </c>
@@ -2094,16 +2095,17 @@
       </c>
       <c r="H48" s="43"/>
     </row>
-    <row r="49" spans="2:25" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="F49" s="25" t="s">
+    <row r="49" spans="2:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="25" t="s">
         <v>34</v>
       </c>
+      <c r="F49" s="25"/>
       <c r="G49" s="50">
         <f>(G48-F7)/F7</f>
         <v>1.2077868064221198E-3</v>
       </c>
     </row>
-    <row r="51" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
       <c r="D51" s="20"/>
@@ -2129,7 +2131,7 @@
       <c r="X51" s="1"/>
       <c r="Y51" s="1"/>
     </row>
-    <row r="52" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -2155,7 +2157,7 @@
       <c r="X52" s="1"/>
       <c r="Y52" s="1"/>
     </row>
-    <row r="53" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
@@ -2181,7 +2183,7 @@
       <c r="X53" s="1"/>
       <c r="Y53" s="1"/>
     </row>
-    <row r="54" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -2207,7 +2209,7 @@
       <c r="X54" s="1"/>
       <c r="Y54" s="1"/>
     </row>
-    <row r="55" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -2233,7 +2235,7 @@
       <c r="X55" s="1"/>
       <c r="Y55" s="1"/>
     </row>
-    <row r="56" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -2259,7 +2261,7 @@
       <c r="X56" s="1"/>
       <c r="Y56" s="1"/>
     </row>
-    <row r="57" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -2285,7 +2287,7 @@
       <c r="X57" s="1"/>
       <c r="Y57" s="1"/>
     </row>
-    <row r="58" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B58" s="57"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -2311,7 +2313,7 @@
       <c r="X58" s="1"/>
       <c r="Y58" s="1"/>
     </row>
-    <row r="59" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -2337,7 +2339,7 @@
       <c r="X59" s="1"/>
       <c r="Y59" s="1"/>
     </row>
-    <row r="60" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
@@ -2363,7 +2365,7 @@
       <c r="X60" s="1"/>
       <c r="Y60" s="1"/>
     </row>
-    <row r="61" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -2389,7 +2391,7 @@
       <c r="X61" s="1"/>
       <c r="Y61" s="1"/>
     </row>
-    <row r="62" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -2415,7 +2417,7 @@
       <c r="X62" s="1"/>
       <c r="Y62" s="1"/>
     </row>
-    <row r="63" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -2441,7 +2443,7 @@
       <c r="X63" s="1"/>
       <c r="Y63" s="1"/>
     </row>
-    <row r="64" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B64" s="57"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -2467,7 +2469,7 @@
       <c r="X64" s="1"/>
       <c r="Y64" s="1"/>
     </row>
-    <row r="65" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -2493,7 +2495,7 @@
       <c r="X65" s="1"/>
       <c r="Y65" s="1"/>
     </row>
-    <row r="66" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
@@ -2519,7 +2521,7 @@
       <c r="X66" s="1"/>
       <c r="Y66" s="1"/>
     </row>
-    <row r="67" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -2545,7 +2547,7 @@
       <c r="X67" s="1"/>
       <c r="Y67" s="1"/>
     </row>
-    <row r="68" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B68" s="57"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -2571,7 +2573,7 @@
       <c r="X68" s="1"/>
       <c r="Y68" s="1"/>
     </row>
-    <row r="69" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -2597,7 +2599,7 @@
       <c r="X69" s="1"/>
       <c r="Y69" s="1"/>
     </row>
-    <row r="70" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -2623,7 +2625,7 @@
       <c r="X70" s="1"/>
       <c r="Y70" s="1"/>
     </row>
-    <row r="71" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B71" s="20"/>
       <c r="C71" s="20"/>
       <c r="D71" s="20"/>
@@ -2649,7 +2651,7 @@
       <c r="X71" s="1"/>
       <c r="Y71" s="1"/>
     </row>
-    <row r="72" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -2675,7 +2677,7 @@
       <c r="X72" s="1"/>
       <c r="Y72" s="1"/>
     </row>
-    <row r="73" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
@@ -2701,7 +2703,7 @@
       <c r="X73" s="1"/>
       <c r="Y73" s="1"/>
     </row>
-    <row r="74" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -2727,7 +2729,7 @@
       <c r="X74" s="1"/>
       <c r="Y74" s="1"/>
     </row>
-    <row r="75" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -2753,7 +2755,7 @@
       <c r="X75" s="1"/>
       <c r="Y75" s="1"/>
     </row>
-    <row r="76" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -2779,7 +2781,7 @@
       <c r="X76" s="1"/>
       <c r="Y76" s="1"/>
     </row>
-    <row r="77" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -2805,7 +2807,7 @@
       <c r="X77" s="1"/>
       <c r="Y77" s="1"/>
     </row>
-    <row r="78" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B78" s="57"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -2831,7 +2833,7 @@
       <c r="X78" s="1"/>
       <c r="Y78" s="1"/>
     </row>
-    <row r="79" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -2857,7 +2859,7 @@
       <c r="X79" s="1"/>
       <c r="Y79" s="1"/>
     </row>
-    <row r="80" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
@@ -2883,7 +2885,7 @@
       <c r="X80" s="1"/>
       <c r="Y80" s="1"/>
     </row>
-    <row r="81" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -2909,7 +2911,7 @@
       <c r="X81" s="1"/>
       <c r="Y81" s="1"/>
     </row>
-    <row r="82" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -2935,7 +2937,7 @@
       <c r="X82" s="1"/>
       <c r="Y82" s="1"/>
     </row>
-    <row r="83" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -2961,7 +2963,7 @@
       <c r="X83" s="1"/>
       <c r="Y83" s="1"/>
     </row>
-    <row r="84" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B84" s="57"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -2987,7 +2989,7 @@
       <c r="X84" s="1"/>
       <c r="Y84" s="1"/>
     </row>
-    <row r="85" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -3013,7 +3015,7 @@
       <c r="X85" s="1"/>
       <c r="Y85" s="1"/>
     </row>
-    <row r="86" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
@@ -3039,7 +3041,7 @@
       <c r="X86" s="1"/>
       <c r="Y86" s="1"/>
     </row>
-    <row r="87" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -3065,7 +3067,7 @@
       <c r="X87" s="1"/>
       <c r="Y87" s="1"/>
     </row>
-    <row r="88" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B88" s="57"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
@@ -3091,7 +3093,7 @@
       <c r="X88" s="1"/>
       <c r="Y88" s="1"/>
     </row>
-    <row r="89" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>

</xml_diff>